<commit_message>
Issue NOL with ER
</commit_message>
<xml_diff>
--- a/src/main/resources/DataProvider/ERHireEducation.xlsx
+++ b/src/main/resources/DataProvider/ERHireEducation.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HadeelSalameh\Desktop\Adek2\src\main\resources\DataProvider\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DC60085-4622-4F45-B026-24B7EE8CEEB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECF0B74F-7227-4944-ACA5-2BE66BE24C72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{0309225A-F2C2-404A-A3FE-7C99E1290A3E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{0309225A-F2C2-404A-A3FE-7C99E1290A3E}"/>
   </bookViews>
   <sheets>
     <sheet name="ER" sheetId="1" r:id="rId1"/>
     <sheet name="ERList" sheetId="2" r:id="rId2"/>
     <sheet name="RequestToChangeER" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>Number of ER</t>
   </si>
@@ -63,6 +65,18 @@
   </si>
   <si>
     <t>Abdulla Khalid</t>
+  </si>
+  <si>
+    <t>Alyazia Khamis</t>
+  </si>
+  <si>
+    <t>Owaisha Aamer</t>
+  </si>
+  <si>
+    <t>er3hadeel@gmail.com</t>
+  </si>
+  <si>
+    <t>ertesting2he@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -428,7 +442,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97CAB526-49B1-446F-A8D9-9BDEC7D620B0}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -458,7 +472,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -480,10 +494,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>8</v>
@@ -491,10 +505,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>8</v>
@@ -502,10 +516,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{558FB573-998F-4D17-8E59-1D7D4A212F88}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{9615F1DE-52AD-4D70-98DA-9DD5B0043D35}"/>
-    <hyperlink ref="C2" r:id="rId3" xr:uid="{73B69DF7-DE3B-4404-8ACB-5A29ADA4BADA}"/>
-    <hyperlink ref="C3" r:id="rId4" xr:uid="{1632543E-E77E-4465-B072-52A3FA851C65}"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{A494F800-08D9-4B00-B8EA-A8507746F444}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{F3C59443-C3E4-4E48-81D8-80A9812EF308}"/>
+    <hyperlink ref="C2" r:id="rId3" xr:uid="{5E0D3F7F-AF9D-4F4B-8962-EEF8CEBE763C}"/>
+    <hyperlink ref="C3" r:id="rId4" xr:uid="{39D42CAE-D4A5-40D8-BFEA-1720EFDD117A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -515,7 +529,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45C4B5B0-52C8-4201-B15D-3ECB0EEB533B}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
@@ -544,4 +558,59 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B0E8EF4-013F-4BA8-A400-8A64E86387FC}">
+  <dimension ref="A2:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{558FB573-998F-4D17-8E59-1D7D4A212F88}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{9615F1DE-52AD-4D70-98DA-9DD5B0043D35}"/>
+    <hyperlink ref="C2" r:id="rId3" xr:uid="{73B69DF7-DE3B-4404-8ACB-5A29ADA4BADA}"/>
+    <hyperlink ref="C3" r:id="rId4" xr:uid="{1632543E-E77E-4465-B072-52A3FA851C65}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F81929C-81BD-4516-B4AC-BF480C375589}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added  ScholarShip Scenarios , removed unwanted files directory : Higher/Education
</commit_message>
<xml_diff>
--- a/src/main/resources/DataProvider/ERHireEducation.xlsx
+++ b/src/main/resources/DataProvider/ERHireEducation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HadeelSalameh\Desktop\Adek2\src\main\resources\DataProvider\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECF0B74F-7227-4944-ACA5-2BE66BE24C72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{263D0618-7622-4F48-B761-1241E3FF07FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{0309225A-F2C2-404A-A3FE-7C99E1290A3E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{0309225A-F2C2-404A-A3FE-7C99E1290A3E}"/>
   </bookViews>
   <sheets>
     <sheet name="ER" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
   <si>
     <t>Number of ER</t>
   </si>
@@ -58,9 +58,6 @@
     <t>Test@123</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>NewERSelection</t>
   </si>
   <si>
@@ -77,6 +74,30 @@
   </si>
   <si>
     <t>ertesting2he@gmail.com</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>ER2@adek.gov.ae</t>
+  </si>
+  <si>
+    <t>ER1@adek.gov.ae</t>
+  </si>
+  <si>
+    <t>ER3@adek.gov.ae</t>
+  </si>
+  <si>
+    <t>Adek@Pas2</t>
+  </si>
+  <si>
+    <t>External Reviewer 1</t>
+  </si>
+  <si>
+    <t>External Reviewers 2</t>
+  </si>
+  <si>
+    <t>External Reviewers 3</t>
   </si>
 </sst>
 </file>
@@ -121,10 +142,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -442,8 +466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97CAB526-49B1-446F-A8D9-9BDEC7D620B0}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -458,7 +482,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -469,10 +493,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E01BFC1-D8F5-4DE3-A01B-3464F818996A}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -494,34 +518,46 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>8</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{A494F800-08D9-4B00-B8EA-A8507746F444}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{F3C59443-C3E4-4E48-81D8-80A9812EF308}"/>
-    <hyperlink ref="C2" r:id="rId3" xr:uid="{5E0D3F7F-AF9D-4F4B-8962-EEF8CEBE763C}"/>
-    <hyperlink ref="C3" r:id="rId4" xr:uid="{39D42CAE-D4A5-40D8-BFEA-1720EFDD117A}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{5E0D3F7F-AF9D-4F4B-8962-EEF8CEBE763C}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{9E6DCF2B-BF4B-4FA7-9856-E5FF8623638E}"/>
+    <hyperlink ref="C3" r:id="rId3" xr:uid="{223A5B66-C41F-4176-9ACD-CE0E51F24F8B}"/>
+    <hyperlink ref="C4" r:id="rId4" xr:uid="{0AA9BD4C-8EC6-4977-AF27-6E438504AC29}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -544,7 +580,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -552,7 +588,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -565,10 +601,13 @@
   <dimension ref="A2:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="27.36328125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -600,17 +639,64 @@
     <hyperlink ref="C3" r:id="rId4" xr:uid="{1632543E-E77E-4465-B072-52A3FA851C65}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F81929C-81BD-4516-B4AC-BF480C375589}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="25.90625" customWidth="1"/>
+    <col min="2" max="2" width="30.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{FB7D98CB-FDCA-4CAA-BAB2-8552FB6B4AE0}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{9A22F398-430E-4AAF-8656-438E328F2976}"/>
+    <hyperlink ref="C2" r:id="rId3" xr:uid="{B0EB2C69-CA9D-47D2-9BA3-572F4A817058}"/>
+    <hyperlink ref="C3" r:id="rId4" xr:uid="{211F8F0A-32D6-4F36-8850-951585922919}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>